<commit_message>
updated without Route 99 owl
</commit_message>
<xml_diff>
--- a/data/raw_data/Owls_Table.xlsx
+++ b/data/raw_data/Owls_Table.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="Owls_Table"/>
   </sheets>
   <definedNames>
-    <definedName name="Owls_Table">'Owls_Table'!$A$1:$J$944</definedName>
+    <definedName name="Owls_Table">'Owls_Table'!$A$1:$J$940</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J944"/>
+  <dimension ref="A1:J940"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -36225,10 +36225,10 @@
     </row>
     <row outlineLevel="0" r="912">
       <c r="A912" s="0">
-        <v>1130</v>
+        <v>1134</v>
       </c>
       <c r="B912" s="0">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C912" s="0" t="inlineStr">
         <is>
@@ -36241,7 +36241,7 @@
         </is>
       </c>
       <c r="E912" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F912" s="0" t="b">
         <v>1</v>
@@ -36250,25 +36250,25 @@
         <v>1</v>
       </c>
       <c r="H912" s="0">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="I912" s="0" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>N</t>
         </is>
       </c>
       <c r="J912" s="0" t="inlineStr">
         <is>
-          <t>Called 2 times</t>
+          <t>Min. 6</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="913">
       <c r="A913" s="0">
-        <v>1131</v>
+        <v>1135</v>
       </c>
       <c r="B913" s="0">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C913" s="0" t="inlineStr">
         <is>
@@ -36284,10 +36284,10 @@
         <v>0</v>
       </c>
       <c r="F913" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G913" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H913" s="0">
         <v>300</v>
@@ -36297,13 +36297,18 @@
           <t>NE</t>
         </is>
       </c>
+      <c r="J913" s="0" t="inlineStr">
+        <is>
+          <t>Minutes 7&amp;7.5; moved to 20 meters NE @ 12 minutes</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="914">
       <c r="A914" s="0">
-        <v>1132</v>
+        <v>1138</v>
       </c>
       <c r="B914" s="0">
-        <v>99</v>
+        <v>903</v>
       </c>
       <c r="C914" s="0" t="inlineStr">
         <is>
@@ -36312,14 +36317,14 @@
       </c>
       <c r="D914" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E914" s="0" t="b">
         <v>0</v>
       </c>
       <c r="F914" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G914" s="0" t="b">
         <v>1</v>
@@ -36329,16 +36334,21 @@
       </c>
       <c r="I914" s="0" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>NE</t>
+        </is>
+      </c>
+      <c r="J914" s="0" t="inlineStr">
+        <is>
+          <t>Min. 6; Called 2 times</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="915">
       <c r="A915" s="0">
-        <v>1133</v>
+        <v>1139</v>
       </c>
       <c r="B915" s="0">
-        <v>99</v>
+        <v>903</v>
       </c>
       <c r="C915" s="0" t="inlineStr">
         <is>
@@ -36347,33 +36357,33 @@
       </c>
       <c r="D915" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E915" s="0" t="b">
         <v>0</v>
       </c>
       <c r="F915" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G915" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H915" s="0">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="I915" s="0" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>NE</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="916">
       <c r="A916" s="0">
-        <v>1134</v>
+        <v>1140</v>
       </c>
       <c r="B916" s="0">
-        <v>97</v>
+        <v>903</v>
       </c>
       <c r="C916" s="0" t="inlineStr">
         <is>
@@ -36382,38 +36392,38 @@
       </c>
       <c r="D916" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E916" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F916" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G916" s="0" t="b">
         <v>1</v>
       </c>
       <c r="H916" s="0">
-        <v>350</v>
+        <v>500</v>
       </c>
       <c r="I916" s="0" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="J916" s="0" t="inlineStr">
         <is>
-          <t>Min. 6</t>
+          <t>Min. 7</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="917">
       <c r="A917" s="0">
-        <v>1135</v>
+        <v>1141</v>
       </c>
       <c r="B917" s="0">
-        <v>97</v>
+        <v>903</v>
       </c>
       <c r="C917" s="0" t="inlineStr">
         <is>
@@ -36422,7 +36432,7 @@
       </c>
       <c r="D917" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E917" s="0" t="b">
@@ -36435,29 +36445,29 @@
         <v>1</v>
       </c>
       <c r="H917" s="0">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="I917" s="0" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>S</t>
         </is>
       </c>
       <c r="J917" s="0" t="inlineStr">
         <is>
-          <t>Minutes 7&amp;7.5; moved to 20 meters NE @ 12 minutes</t>
+          <t>Min. 8</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="918">
       <c r="A918" s="0">
-        <v>1138</v>
+        <v>1142</v>
       </c>
       <c r="B918" s="0">
-        <v>903</v>
+        <v>239</v>
       </c>
       <c r="C918" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D918" s="0" t="inlineStr">
@@ -36469,75 +36479,60 @@
         <v>0</v>
       </c>
       <c r="F918" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G918" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H918" s="0">
-        <v>500</v>
-      </c>
-      <c r="I918" s="0" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
-      </c>
-      <c r="J918" s="0" t="inlineStr">
-        <is>
-          <t>Min. 6; Called 2 times</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row outlineLevel="0" r="919">
       <c r="A919" s="0">
-        <v>1139</v>
+        <v>1143</v>
       </c>
       <c r="B919" s="0">
-        <v>903</v>
+        <v>240</v>
       </c>
       <c r="C919" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D919" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E919" s="0" t="b">
         <v>0</v>
       </c>
       <c r="F919" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G919" s="0" t="b">
         <v>0</v>
       </c>
       <c r="H919" s="0">
-        <v>300</v>
-      </c>
-      <c r="I919" s="0" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row outlineLevel="0" r="920">
       <c r="A920" s="0">
-        <v>1140</v>
+        <v>1144</v>
       </c>
       <c r="B920" s="0">
-        <v>903</v>
+        <v>352</v>
       </c>
       <c r="C920" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D920" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E920" s="0" t="b">
@@ -36547,37 +36542,32 @@
         <v>0</v>
       </c>
       <c r="G920" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H920" s="0">
-        <v>500</v>
-      </c>
-      <c r="I920" s="0" t="inlineStr">
-        <is>
-          <t>SE</t>
-        </is>
+        <v>0</v>
       </c>
       <c r="J920" s="0" t="inlineStr">
         <is>
-          <t>Min. 7</t>
+          <t>No owls vocalizing at survey points.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="921">
       <c r="A921" s="0">
-        <v>1141</v>
+        <v>1145</v>
       </c>
       <c r="B921" s="0">
-        <v>903</v>
+        <v>362</v>
       </c>
       <c r="C921" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D921" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E921" s="0" t="b">
@@ -36587,28 +36577,23 @@
         <v>0</v>
       </c>
       <c r="G921" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H921" s="0">
-        <v>600</v>
-      </c>
-      <c r="I921" s="0" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
+        <v>0</v>
       </c>
       <c r="J921" s="0" t="inlineStr">
         <is>
-          <t>Min. 8</t>
+          <t>No owls heard at survey points on transect.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="922">
       <c r="A922" s="0">
-        <v>1142</v>
+        <v>1146</v>
       </c>
       <c r="B922" s="0">
-        <v>239</v>
+        <v>512</v>
       </c>
       <c r="C922" s="0" t="inlineStr">
         <is>
@@ -36631,48 +36616,63 @@
       </c>
       <c r="H922" s="0">
         <v>0</v>
+      </c>
+      <c r="J922" s="0" t="inlineStr">
+        <is>
+          <t>No owls vocalized at survey points</t>
+        </is>
       </c>
     </row>
     <row outlineLevel="0" r="923">
       <c r="A923" s="0">
-        <v>1143</v>
+        <v>1148</v>
       </c>
       <c r="B923" s="0">
-        <v>240</v>
+        <v>117</v>
       </c>
       <c r="C923" s="0" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>NoID</t>
         </is>
       </c>
       <c r="D923" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E923" s="0" t="b">
         <v>0</v>
       </c>
       <c r="F923" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G923" s="0" t="b">
         <v>0</v>
       </c>
       <c r="H923" s="0">
         <v>0</v>
+      </c>
+      <c r="I923" s="0" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="J923" s="0" t="inlineStr">
+        <is>
+          <t>Single hoot long ways off</t>
+        </is>
       </c>
     </row>
     <row outlineLevel="0" r="924">
       <c r="A924" s="0">
-        <v>1144</v>
+        <v>1149</v>
       </c>
       <c r="B924" s="0">
-        <v>352</v>
+        <v>109</v>
       </c>
       <c r="C924" s="0" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Mottd</t>
         </is>
       </c>
       <c r="D924" s="0" t="inlineStr">
@@ -36687,27 +36687,32 @@
         <v>0</v>
       </c>
       <c r="G924" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H924" s="0">
-        <v>0</v>
+        <v>250</v>
+      </c>
+      <c r="I924" s="0" t="inlineStr">
+        <is>
+          <t>SW</t>
+        </is>
       </c>
       <c r="J924" s="0" t="inlineStr">
         <is>
-          <t>No owls vocalizing at survey points.</t>
+          <t>Min. 11-12; started w/ normal vocalization</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="925">
       <c r="A925" s="0">
-        <v>1145</v>
+        <v>1150</v>
       </c>
       <c r="B925" s="0">
-        <v>362</v>
+        <v>162</v>
       </c>
       <c r="C925" s="0" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Mottd</t>
         </is>
       </c>
       <c r="D925" s="0" t="inlineStr">
@@ -36719,35 +36724,40 @@
         <v>0</v>
       </c>
       <c r="F925" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G925" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H925" s="0">
-        <v>0</v>
+        <v>400</v>
+      </c>
+      <c r="I925" s="0" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
       <c r="J925" s="0" t="inlineStr">
         <is>
-          <t>No owls heard at survey points on transect.</t>
+          <t>Min 6 plus; other side of the river</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="926">
       <c r="A926" s="0">
-        <v>1146</v>
+        <v>1151</v>
       </c>
       <c r="B926" s="0">
-        <v>512</v>
+        <v>162</v>
       </c>
       <c r="C926" s="0" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Mottd</t>
         </is>
       </c>
       <c r="D926" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E926" s="0" t="b">
@@ -36757,63 +36767,68 @@
         <v>0</v>
       </c>
       <c r="G926" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H926" s="0">
-        <v>0</v>
+        <v>300</v>
+      </c>
+      <c r="I926" s="0" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
       </c>
       <c r="J926" s="0" t="inlineStr">
         <is>
-          <t>No owls vocalized at survey points</t>
+          <t>Min 8 plus;</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="927">
       <c r="A927" s="0">
-        <v>1148</v>
+        <v>1152</v>
       </c>
       <c r="B927" s="0">
-        <v>117</v>
+        <v>163</v>
       </c>
       <c r="C927" s="0" t="inlineStr">
         <is>
-          <t>NoID</t>
+          <t>Specd</t>
         </is>
       </c>
       <c r="D927" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E927" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F927" s="0" t="b">
         <v>1</v>
       </c>
       <c r="G927" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H927" s="0">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I927" s="0" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
       <c r="J927" s="0" t="inlineStr">
         <is>
-          <t>Single hoot long ways off</t>
+          <t>Min 6 plus</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="928">
       <c r="A928" s="0">
-        <v>1149</v>
+        <v>1153</v>
       </c>
       <c r="B928" s="0">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="C928" s="0" t="inlineStr">
         <is>
@@ -36822,38 +36837,38 @@
       </c>
       <c r="D928" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E928" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F928" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G928" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H928" s="0">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="I928" s="0" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>S</t>
         </is>
       </c>
       <c r="J928" s="0" t="inlineStr">
         <is>
-          <t>Min. 11-12; started w/ normal vocalization</t>
+          <t>Min 5 plus</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="929">
       <c r="A929" s="0">
-        <v>1150</v>
+        <v>1154</v>
       </c>
       <c r="B929" s="0">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C929" s="0" t="inlineStr">
         <is>
@@ -36862,20 +36877,20 @@
       </c>
       <c r="D929" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E929" s="0" t="b">
         <v>0</v>
       </c>
       <c r="F929" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G929" s="0" t="b">
         <v>1</v>
       </c>
       <c r="H929" s="0">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="I929" s="0" t="inlineStr">
         <is>
@@ -36884,25 +36899,25 @@
       </c>
       <c r="J929" s="0" t="inlineStr">
         <is>
-          <t>Min 6 plus; other side of the river</t>
+          <t>Min 5 plus; Across river</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="930">
       <c r="A930" s="0">
-        <v>1151</v>
+        <v>1155</v>
       </c>
       <c r="B930" s="0">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C930" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>Specd</t>
         </is>
       </c>
       <c r="D930" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E930" s="0" t="b">
@@ -36915,7 +36930,7 @@
         <v>1</v>
       </c>
       <c r="H930" s="0">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="I930" s="0" t="inlineStr">
         <is>
@@ -36924,20 +36939,20 @@
       </c>
       <c r="J930" s="0" t="inlineStr">
         <is>
-          <t>Min 8 plus;</t>
+          <t>Min 6 plus</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="931">
       <c r="A931" s="0">
-        <v>1152</v>
+        <v>1156</v>
       </c>
       <c r="B931" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C931" s="0" t="inlineStr">
         <is>
-          <t>Specd</t>
+          <t>Mottd</t>
         </is>
       </c>
       <c r="D931" s="0" t="inlineStr">
@@ -36946,13 +36961,13 @@
         </is>
       </c>
       <c r="E931" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F931" s="0" t="b">
         <v>1</v>
       </c>
       <c r="G931" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H931" s="0">
         <v>200</v>
@@ -36962,18 +36977,13 @@
           <t>S</t>
         </is>
       </c>
-      <c r="J931" s="0" t="inlineStr">
-        <is>
-          <t>Min 6 plus</t>
-        </is>
-      </c>
     </row>
     <row outlineLevel="0" r="932">
       <c r="A932" s="0">
-        <v>1153</v>
+        <v>1157</v>
       </c>
       <c r="B932" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C932" s="0" t="inlineStr">
         <is>
@@ -36986,38 +36996,38 @@
         </is>
       </c>
       <c r="E932" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F932" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G932" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H932" s="0">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="I932" s="0" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="J932" s="0" t="inlineStr">
         <is>
-          <t>Min 5 plus</t>
+          <t>Min 5; Across river</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="933">
       <c r="A933" s="0">
-        <v>1154</v>
+        <v>1158</v>
       </c>
       <c r="B933" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C933" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>Specd</t>
         </is>
       </c>
       <c r="D933" s="0" t="inlineStr">
@@ -37035,25 +37045,25 @@
         <v>1</v>
       </c>
       <c r="H933" s="0">
-        <v>450</v>
+        <v>150</v>
       </c>
       <c r="I933" s="0" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="J933" s="0" t="inlineStr">
         <is>
-          <t>Min 5 plus; Across river</t>
+          <t>Min 6 plus; this opposite direction from pt. 7 toward pt.9</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="934">
       <c r="A934" s="0">
-        <v>1155</v>
+        <v>1159</v>
       </c>
       <c r="B934" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C934" s="0" t="inlineStr">
         <is>
@@ -37075,7 +37085,7 @@
         <v>1</v>
       </c>
       <c r="H934" s="0">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="I934" s="0" t="inlineStr">
         <is>
@@ -37084,20 +37094,20 @@
       </c>
       <c r="J934" s="0" t="inlineStr">
         <is>
-          <t>Min 6 plus</t>
+          <t>Min 6 plus; one from point 7</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="935">
       <c r="A935" s="0">
-        <v>1156</v>
+        <v>1160</v>
       </c>
       <c r="B935" s="0">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C935" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>Specd</t>
         </is>
       </c>
       <c r="D935" s="0" t="inlineStr">
@@ -37106,33 +37116,38 @@
         </is>
       </c>
       <c r="E935" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F935" s="0" t="b">
         <v>1</v>
       </c>
       <c r="G935" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H935" s="0">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="I935" s="0" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="J935" s="0" t="inlineStr">
+        <is>
+          <t>Min 5 plus</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="936">
       <c r="A936" s="0">
-        <v>1157</v>
+        <v>1161</v>
       </c>
       <c r="B936" s="0">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C936" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>Specd</t>
         </is>
       </c>
       <c r="D936" s="0" t="inlineStr">
@@ -37141,38 +37156,38 @@
         </is>
       </c>
       <c r="E936" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F936" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G936" s="0" t="b">
         <v>1</v>
       </c>
       <c r="H936" s="0">
-        <v>400</v>
+        <v>150</v>
       </c>
       <c r="I936" s="0" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="J936" s="0" t="inlineStr">
         <is>
-          <t>Min 5; Across river</t>
+          <t>Min 10 &amp; 12</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="937">
       <c r="A937" s="0">
-        <v>1158</v>
+        <v>1162</v>
       </c>
       <c r="B937" s="0">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C937" s="0" t="inlineStr">
         <is>
-          <t>Specd</t>
+          <t>Mottd</t>
         </is>
       </c>
       <c r="D937" s="0" t="inlineStr">
@@ -37190,25 +37205,25 @@
         <v>1</v>
       </c>
       <c r="H937" s="0">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="I937" s="0" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="J937" s="0" t="inlineStr">
         <is>
-          <t>Min 6 plus; this opposite direction from pt. 7 toward pt.9</t>
+          <t>Min 5; across river</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="938">
       <c r="A938" s="0">
-        <v>1159</v>
+        <v>1163</v>
       </c>
       <c r="B938" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C938" s="0" t="inlineStr">
         <is>
@@ -37217,42 +37232,42 @@
       </c>
       <c r="D938" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E938" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F938" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G938" s="0" t="b">
         <v>1</v>
       </c>
       <c r="H938" s="0">
-        <v>250</v>
+        <v>75</v>
       </c>
       <c r="I938" s="0" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>E</t>
         </is>
       </c>
       <c r="J938" s="0" t="inlineStr">
         <is>
-          <t>Min 6 plus; one from point 7</t>
+          <t>Min 3 plus</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="939">
       <c r="A939" s="0">
-        <v>1160</v>
+        <v>1164</v>
       </c>
       <c r="B939" s="0">
-        <v>165</v>
+        <v>297</v>
       </c>
       <c r="C939" s="0" t="inlineStr">
         <is>
-          <t>Specd</t>
+          <t>Mottd</t>
         </is>
       </c>
       <c r="D939" s="0" t="inlineStr">
@@ -37267,32 +37282,22 @@
         <v>1</v>
       </c>
       <c r="G939" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H939" s="0">
-        <v>150</v>
-      </c>
-      <c r="I939" s="0" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="J939" s="0" t="inlineStr">
-        <is>
-          <t>Min 5 plus</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row outlineLevel="0" r="940">
       <c r="A940" s="0">
-        <v>1161</v>
+        <v>1165</v>
       </c>
       <c r="B940" s="0">
-        <v>165</v>
+        <v>297</v>
       </c>
       <c r="C940" s="0" t="inlineStr">
         <is>
-          <t>Specd</t>
+          <t>Mottd</t>
         </is>
       </c>
       <c r="D940" s="0" t="inlineStr">
@@ -37301,7 +37306,7 @@
         </is>
       </c>
       <c r="E940" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F940" s="0" t="b">
         <v>1</v>
@@ -37310,159 +37315,9 @@
         <v>1</v>
       </c>
       <c r="H940" s="0">
-        <v>150</v>
-      </c>
-      <c r="I940" s="0" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
+        <v>0</v>
       </c>
       <c r="J940" s="0" t="inlineStr">
-        <is>
-          <t>Min 10 &amp; 12</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="941">
-      <c r="A941" s="0">
-        <v>1162</v>
-      </c>
-      <c r="B941" s="0">
-        <v>165</v>
-      </c>
-      <c r="C941" s="0" t="inlineStr">
-        <is>
-          <t>Mottd</t>
-        </is>
-      </c>
-      <c r="D941" s="0" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E941" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="F941" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="G941" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="H941" s="0">
-        <v>400</v>
-      </c>
-      <c r="I941" s="0" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="J941" s="0" t="inlineStr">
-        <is>
-          <t>Min 5; across river</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="942">
-      <c r="A942" s="0">
-        <v>1163</v>
-      </c>
-      <c r="B942" s="0">
-        <v>166</v>
-      </c>
-      <c r="C942" s="0" t="inlineStr">
-        <is>
-          <t>Specd</t>
-        </is>
-      </c>
-      <c r="D942" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E942" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="F942" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="G942" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="H942" s="0">
-        <v>75</v>
-      </c>
-      <c r="I942" s="0" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="J942" s="0" t="inlineStr">
-        <is>
-          <t>Min 3 plus</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="943">
-      <c r="A943" s="0">
-        <v>1164</v>
-      </c>
-      <c r="B943" s="0">
-        <v>297</v>
-      </c>
-      <c r="C943" s="0" t="inlineStr">
-        <is>
-          <t>Mottd</t>
-        </is>
-      </c>
-      <c r="D943" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E943" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="F943" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="G943" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="H943" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="944">
-      <c r="A944" s="0">
-        <v>1165</v>
-      </c>
-      <c r="B944" s="0">
-        <v>297</v>
-      </c>
-      <c r="C944" s="0" t="inlineStr">
-        <is>
-          <t>Mottd</t>
-        </is>
-      </c>
-      <c r="D944" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E944" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="F944" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="G944" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="H944" s="0">
-        <v>0</v>
-      </c>
-      <c r="J944" s="0" t="inlineStr">
         <is>
           <t>Min 7 plus</t>
         </is>

</xml_diff>